<commit_message>
Updated Resident Services Privileges
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Roles and Responsibility_Matrix_16Jan19.xlsx
+++ b/requirements/MOSIP_Roles and Responsibility_Matrix_16Jan19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A60DA7D7-6ACA-4CFA-B7FE-05498769A0C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EF788ED8-76B7-4A66-9289-2C5DE037A0B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2184,12 +2184,120 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="15" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2208,6 +2316,9 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2223,121 +2334,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="15" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2633,7 +2633,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="210" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="172" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="13" customWidth="1"/>
     <col min="3" max="3" width="78.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="9" customWidth="1"/>
@@ -2653,40 +2653,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:309" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="213" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="173" t="s">
+      <c r="B1" s="209" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="211" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="173" t="s">
+      <c r="D1" s="209" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="173" t="s">
+      <c r="E1" s="209" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="174" t="s">
+      <c r="F1" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="179" t="s">
+      <c r="G1" s="216" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="171" t="s">
+      <c r="H1" s="217"/>
+      <c r="I1" s="217"/>
+      <c r="J1" s="217"/>
+      <c r="K1" s="217"/>
+      <c r="L1" s="217"/>
+      <c r="M1" s="217"/>
+      <c r="N1" s="217"/>
+      <c r="O1" s="217"/>
+      <c r="P1" s="203" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="172"/>
-      <c r="R1" s="172"/>
+      <c r="Q1" s="204"/>
+      <c r="R1" s="204"/>
       <c r="S1" s="24"/>
       <c r="T1" s="15"/>
       <c r="U1" s="15"/>
@@ -2761,12 +2761,12 @@
       <c r="CL1" s="21"/>
     </row>
     <row r="2" spans="1:309" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="178"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
+      <c r="A2" s="214"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
       <c r="G2" s="45" t="s">
         <v>8</v>
       </c>
@@ -2877,10 +2877,10 @@
       <c r="CL2" s="21"/>
     </row>
     <row r="3" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="187" t="s">
+      <c r="B3" s="190" t="s">
         <v>138</v>
       </c>
       <c r="C3" s="93"/>
@@ -2993,8 +2993,8 @@
       <c r="CL3" s="20"/>
     </row>
     <row r="4" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="196"/>
-      <c r="B4" s="188"/>
+      <c r="A4" s="185"/>
+      <c r="B4" s="191"/>
       <c r="C4" s="94"/>
       <c r="D4" s="12"/>
       <c r="E4" s="92"/>
@@ -3105,7 +3105,7 @@
       <c r="CL4" s="20"/>
     </row>
     <row r="5" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="196"/>
+      <c r="A5" s="185"/>
       <c r="B5" s="89" t="s">
         <v>151</v>
       </c>
@@ -3219,7 +3219,7 @@
       <c r="CL5" s="20"/>
     </row>
     <row r="6" spans="1:309" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="196"/>
+      <c r="A6" s="185"/>
       <c r="B6" s="89" t="s">
         <v>137</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="CL6" s="20"/>
     </row>
     <row r="7" spans="1:309" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="196"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="89" t="s">
         <v>139</v>
       </c>
@@ -3447,8 +3447,8 @@
       <c r="CL7" s="20"/>
     </row>
     <row r="8" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
-      <c r="B8" s="188" t="s">
+      <c r="A8" s="185"/>
+      <c r="B8" s="191" t="s">
         <v>147</v>
       </c>
       <c r="C8" s="94" t="s">
@@ -3549,8 +3549,8 @@
       <c r="CL8" s="20"/>
     </row>
     <row r="9" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="196"/>
-      <c r="B9" s="188"/>
+      <c r="A9" s="185"/>
+      <c r="B9" s="191"/>
       <c r="C9" s="94" t="s">
         <v>153</v>
       </c>
@@ -3649,8 +3649,8 @@
       <c r="CL9" s="20"/>
     </row>
     <row r="10" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="196"/>
-      <c r="B10" s="188"/>
+      <c r="A10" s="185"/>
+      <c r="B10" s="191"/>
       <c r="C10" s="94" t="s">
         <v>154</v>
       </c>
@@ -3749,7 +3749,7 @@
       <c r="CL10" s="20"/>
     </row>
     <row r="11" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="196"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="89" t="s">
         <v>117</v>
       </c>
@@ -3849,7 +3849,7 @@
       <c r="CL11" s="20"/>
     </row>
     <row r="12" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="196"/>
+      <c r="A12" s="185"/>
       <c r="B12" s="89" t="s">
         <v>146</v>
       </c>
@@ -3945,7 +3945,7 @@
       <c r="CL12" s="20"/>
     </row>
     <row r="13" spans="1:309" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="197"/>
+      <c r="A13" s="186"/>
       <c r="B13" s="29" t="s">
         <v>145</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="CL13" s="20"/>
     </row>
     <row r="14" spans="1:309" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="198" t="s">
+      <c r="A14" s="205" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="90" t="s">
@@ -4141,7 +4141,7 @@
       <c r="CL14" s="20"/>
     </row>
     <row r="15" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="199"/>
+      <c r="A15" s="206"/>
       <c r="B15" s="56"/>
       <c r="C15" s="100" t="s">
         <v>156</v>
@@ -4456,7 +4456,7 @@
       <c r="KW15" s="12"/>
     </row>
     <row r="16" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="199"/>
+      <c r="A16" s="206"/>
       <c r="B16" s="82"/>
       <c r="C16" s="14" t="s">
         <v>157</v>
@@ -4771,7 +4771,7 @@
       <c r="KW16" s="12"/>
     </row>
     <row r="17" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="199"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="82"/>
       <c r="C17" s="14" t="s">
         <v>158</v>
@@ -5086,7 +5086,7 @@
       <c r="KW17" s="12"/>
     </row>
     <row r="18" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="199"/>
+      <c r="A18" s="206"/>
       <c r="B18" s="82"/>
       <c r="C18" s="14" t="s">
         <v>159</v>
@@ -5401,7 +5401,7 @@
       <c r="KW18" s="12"/>
     </row>
     <row r="19" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="199"/>
+      <c r="A19" s="206"/>
       <c r="B19" s="82"/>
       <c r="C19" s="14" t="s">
         <v>160</v>
@@ -5716,7 +5716,7 @@
       <c r="KW19" s="12"/>
     </row>
     <row r="20" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="199"/>
+      <c r="A20" s="206"/>
       <c r="B20" s="82"/>
       <c r="C20" s="100" t="s">
         <v>161</v>
@@ -6031,7 +6031,7 @@
       <c r="KW20" s="12"/>
     </row>
     <row r="21" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="199"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="82"/>
       <c r="C21" s="14" t="s">
         <v>162</v>
@@ -6346,7 +6346,7 @@
       <c r="KW21" s="12"/>
     </row>
     <row r="22" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="199"/>
+      <c r="A22" s="206"/>
       <c r="B22" s="82"/>
       <c r="C22" s="14" t="s">
         <v>163</v>
@@ -6661,7 +6661,7 @@
       <c r="KW22" s="12"/>
     </row>
     <row r="23" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="199"/>
+      <c r="A23" s="206"/>
       <c r="B23" s="82"/>
       <c r="C23" s="14" t="s">
         <v>164</v>
@@ -6976,7 +6976,7 @@
       <c r="KW23" s="12"/>
     </row>
     <row r="24" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="199"/>
+      <c r="A24" s="206"/>
       <c r="B24" s="82"/>
       <c r="C24" s="100" t="s">
         <v>165</v>
@@ -7291,7 +7291,7 @@
       <c r="KW24" s="12"/>
     </row>
     <row r="25" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="199"/>
+      <c r="A25" s="206"/>
       <c r="B25" s="82"/>
       <c r="C25" s="100" t="s">
         <v>166</v>
@@ -7606,7 +7606,7 @@
       <c r="KW25" s="12"/>
     </row>
     <row r="26" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="199"/>
+      <c r="A26" s="206"/>
       <c r="B26" s="82"/>
       <c r="C26" s="100" t="s">
         <v>167</v>
@@ -7921,7 +7921,7 @@
       <c r="KW26" s="12"/>
     </row>
     <row r="27" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="199"/>
+      <c r="A27" s="206"/>
       <c r="B27" s="82"/>
       <c r="C27" s="100" t="s">
         <v>168</v>
@@ -8236,7 +8236,7 @@
       <c r="KW27" s="12"/>
     </row>
     <row r="28" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="199"/>
+      <c r="A28" s="206"/>
       <c r="B28" s="82"/>
       <c r="C28" s="100" t="s">
         <v>169</v>
@@ -8551,7 +8551,7 @@
       <c r="KW28" s="12"/>
     </row>
     <row r="29" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="199"/>
+      <c r="A29" s="206"/>
       <c r="B29" s="82"/>
       <c r="C29" s="100" t="s">
         <v>170</v>
@@ -8866,7 +8866,7 @@
       <c r="KW29" s="12"/>
     </row>
     <row r="30" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="199"/>
+      <c r="A30" s="206"/>
       <c r="B30" s="82"/>
       <c r="C30" s="100" t="s">
         <v>171</v>
@@ -9181,7 +9181,7 @@
       <c r="KW30" s="12"/>
     </row>
     <row r="31" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="199"/>
+      <c r="A31" s="206"/>
       <c r="B31" s="82"/>
       <c r="C31" s="100" t="s">
         <v>172</v>
@@ -9496,7 +9496,7 @@
       <c r="KW31" s="12"/>
     </row>
     <row r="32" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="199"/>
+      <c r="A32" s="206"/>
       <c r="B32" s="82"/>
       <c r="C32" s="100" t="s">
         <v>173</v>
@@ -9811,7 +9811,7 @@
       <c r="KW32" s="12"/>
     </row>
     <row r="33" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="199"/>
+      <c r="A33" s="206"/>
       <c r="B33" s="82"/>
       <c r="C33" s="100" t="s">
         <v>174</v>
@@ -10126,7 +10126,7 @@
       <c r="KW33" s="12"/>
     </row>
     <row r="34" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="199"/>
+      <c r="A34" s="206"/>
       <c r="B34" s="82"/>
       <c r="C34" s="100" t="s">
         <v>175</v>
@@ -10441,7 +10441,7 @@
       <c r="KW34" s="12"/>
     </row>
     <row r="35" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="199"/>
+      <c r="A35" s="206"/>
       <c r="B35" s="82"/>
       <c r="C35" s="100" t="s">
         <v>176</v>
@@ -10756,7 +10756,7 @@
       <c r="KW35" s="12"/>
     </row>
     <row r="36" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="199"/>
+      <c r="A36" s="206"/>
       <c r="B36" s="82"/>
       <c r="C36" s="100" t="s">
         <v>177</v>
@@ -11071,7 +11071,7 @@
       <c r="KW36" s="12"/>
     </row>
     <row r="37" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="199"/>
+      <c r="A37" s="206"/>
       <c r="B37" s="82"/>
       <c r="C37" s="100" t="s">
         <v>178</v>
@@ -11386,7 +11386,7 @@
       <c r="KW37" s="12"/>
     </row>
     <row r="38" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="199"/>
+      <c r="A38" s="206"/>
       <c r="B38" s="82"/>
       <c r="C38" s="100" t="s">
         <v>179</v>
@@ -11701,7 +11701,7 @@
       <c r="KW38" s="12"/>
     </row>
     <row r="39" spans="1:309" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="199"/>
+      <c r="A39" s="206"/>
       <c r="B39" s="82"/>
       <c r="C39" s="100" t="s">
         <v>180</v>
@@ -12016,7 +12016,7 @@
       <c r="KW39" s="12"/>
     </row>
     <row r="40" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A40" s="199"/>
+      <c r="A40" s="206"/>
       <c r="B40" s="56" t="s">
         <v>20</v>
       </c>
@@ -12078,7 +12078,7 @@
       <c r="BY40" s="10"/>
     </row>
     <row r="41" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A41" s="199"/>
+      <c r="A41" s="206"/>
       <c r="B41" s="56" t="s">
         <v>127</v>
       </c>
@@ -12140,7 +12140,7 @@
       <c r="BY41" s="10"/>
     </row>
     <row r="42" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A42" s="199"/>
+      <c r="A42" s="206"/>
       <c r="B42" s="88" t="s">
         <v>136</v>
       </c>
@@ -12200,7 +12200,7 @@
       <c r="BY42" s="10"/>
     </row>
     <row r="43" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A43" s="199"/>
+      <c r="A43" s="206"/>
       <c r="B43" s="55" t="s">
         <v>128</v>
       </c>
@@ -12262,8 +12262,8 @@
       <c r="BY43" s="10"/>
     </row>
     <row r="44" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A44" s="199"/>
-      <c r="B44" s="189" t="s">
+      <c r="A44" s="206"/>
+      <c r="B44" s="192" t="s">
         <v>129</v>
       </c>
       <c r="C44" s="98" t="s">
@@ -12324,8 +12324,8 @@
       <c r="BY44" s="10"/>
     </row>
     <row r="45" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A45" s="199"/>
-      <c r="B45" s="190"/>
+      <c r="A45" s="206"/>
+      <c r="B45" s="193"/>
       <c r="C45" s="98" t="s">
         <v>185</v>
       </c>
@@ -12384,8 +12384,8 @@
       <c r="BY45" s="10"/>
     </row>
     <row r="46" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A46" s="199"/>
-      <c r="B46" s="190"/>
+      <c r="A46" s="206"/>
+      <c r="B46" s="193"/>
       <c r="C46" s="98" t="s">
         <v>186</v>
       </c>
@@ -12444,8 +12444,8 @@
       <c r="BY46" s="10"/>
     </row>
     <row r="47" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A47" s="199"/>
-      <c r="B47" s="190"/>
+      <c r="A47" s="206"/>
+      <c r="B47" s="193"/>
       <c r="C47" s="98" t="s">
         <v>187</v>
       </c>
@@ -12504,8 +12504,8 @@
       <c r="BY47" s="10"/>
     </row>
     <row r="48" spans="1:309" x14ac:dyDescent="0.25">
-      <c r="A48" s="199"/>
-      <c r="B48" s="191"/>
+      <c r="A48" s="206"/>
+      <c r="B48" s="194"/>
       <c r="C48" s="98" t="s">
         <v>188</v>
       </c>
@@ -12564,7 +12564,7 @@
       <c r="BY48" s="10"/>
     </row>
     <row r="49" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A49" s="199"/>
+      <c r="A49" s="206"/>
       <c r="B49" s="55" t="s">
         <v>131</v>
       </c>
@@ -12626,7 +12626,7 @@
       <c r="BY49" s="10"/>
     </row>
     <row r="50" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A50" s="199"/>
+      <c r="A50" s="206"/>
       <c r="B50" s="55" t="s">
         <v>132</v>
       </c>
@@ -12688,7 +12688,7 @@
       <c r="BY50" s="10"/>
     </row>
     <row r="51" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A51" s="199"/>
+      <c r="A51" s="206"/>
       <c r="B51" s="55" t="s">
         <v>134</v>
       </c>
@@ -12750,7 +12750,7 @@
       <c r="BY51" s="10"/>
     </row>
     <row r="52" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A52" s="199"/>
+      <c r="A52" s="206"/>
       <c r="B52" s="55" t="s">
         <v>133</v>
       </c>
@@ -12810,7 +12810,7 @@
       <c r="BY52" s="10"/>
     </row>
     <row r="53" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A53" s="199"/>
+      <c r="A53" s="206"/>
       <c r="B53" s="55" t="s">
         <v>135</v>
       </c>
@@ -12870,7 +12870,7 @@
       <c r="BY53" s="10"/>
     </row>
     <row r="54" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="200"/>
+      <c r="A54" s="215"/>
       <c r="B54" s="29" t="s">
         <v>130</v>
       </c>
@@ -12930,17 +12930,17 @@
       <c r="BY54" s="10"/>
     </row>
     <row r="55" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="198" t="s">
+      <c r="A55" s="205" t="s">
         <v>21</v>
       </c>
       <c r="B55" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C55" s="194" t="s">
+      <c r="C55" s="198" t="s">
         <v>23</v>
       </c>
       <c r="D55" s="28"/>
-      <c r="E55" s="192"/>
+      <c r="E55" s="195"/>
       <c r="F55" s="65" t="s">
         <v>24</v>
       </c>
@@ -13018,11 +13018,11 @@
       </c>
     </row>
     <row r="56" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="199"/>
+      <c r="A56" s="206"/>
       <c r="B56" s="56"/>
-      <c r="C56" s="184"/>
+      <c r="C56" s="197"/>
       <c r="D56" s="12"/>
-      <c r="E56" s="193"/>
+      <c r="E56" s="196"/>
       <c r="F56" s="66" t="s">
         <v>25</v>
       </c>
@@ -13076,11 +13076,11 @@
       <c r="BY56" s="10"/>
     </row>
     <row r="57" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="199"/>
+      <c r="A57" s="206"/>
       <c r="B57" s="56"/>
-      <c r="C57" s="184"/>
+      <c r="C57" s="197"/>
       <c r="D57" s="12"/>
-      <c r="E57" s="193"/>
+      <c r="E57" s="196"/>
       <c r="F57" s="66" t="s">
         <v>26</v>
       </c>
@@ -13136,11 +13136,11 @@
       <c r="BY57" s="10"/>
     </row>
     <row r="58" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="199"/>
+      <c r="A58" s="206"/>
       <c r="B58" s="56"/>
-      <c r="C58" s="184"/>
+      <c r="C58" s="197"/>
       <c r="D58" s="12"/>
-      <c r="E58" s="193"/>
+      <c r="E58" s="196"/>
       <c r="F58" s="125" t="s">
         <v>27</v>
       </c>
@@ -13196,9 +13196,9 @@
       <c r="BY58" s="10"/>
     </row>
     <row r="59" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="199"/>
+      <c r="A59" s="206"/>
       <c r="B59" s="56"/>
-      <c r="C59" s="184" t="s">
+      <c r="C59" s="197" t="s">
         <v>28</v>
       </c>
       <c r="D59" s="12"/>
@@ -13258,9 +13258,9 @@
       <c r="BY59" s="10"/>
     </row>
     <row r="60" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="199"/>
+      <c r="A60" s="206"/>
       <c r="B60" s="56"/>
-      <c r="C60" s="184"/>
+      <c r="C60" s="197"/>
       <c r="D60" s="12"/>
       <c r="E60" s="68"/>
       <c r="F60" s="66" t="s">
@@ -13318,9 +13318,9 @@
       <c r="BY60" s="10"/>
     </row>
     <row r="61" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="199"/>
+      <c r="A61" s="206"/>
       <c r="B61" s="56"/>
-      <c r="C61" s="184"/>
+      <c r="C61" s="197"/>
       <c r="D61" s="12"/>
       <c r="E61" s="68"/>
       <c r="F61" s="66" t="s">
@@ -13378,9 +13378,9 @@
       <c r="BY61" s="10"/>
     </row>
     <row r="62" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="199"/>
+      <c r="A62" s="206"/>
       <c r="B62" s="56"/>
-      <c r="C62" s="184" t="s">
+      <c r="C62" s="197" t="s">
         <v>32</v>
       </c>
       <c r="D62" s="12"/>
@@ -13440,9 +13440,9 @@
       <c r="BY62" s="10"/>
     </row>
     <row r="63" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="199"/>
+      <c r="A63" s="206"/>
       <c r="B63" s="56"/>
-      <c r="C63" s="184"/>
+      <c r="C63" s="197"/>
       <c r="D63" s="12"/>
       <c r="E63" s="68"/>
       <c r="F63" s="66" t="s">
@@ -13500,9 +13500,9 @@
       <c r="BY63" s="10"/>
     </row>
     <row r="64" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="199"/>
+      <c r="A64" s="206"/>
       <c r="B64" s="56"/>
-      <c r="C64" s="184"/>
+      <c r="C64" s="197"/>
       <c r="D64" s="12"/>
       <c r="E64" s="68"/>
       <c r="F64" s="66" t="s">
@@ -13560,9 +13560,9 @@
       <c r="BY64" s="10"/>
     </row>
     <row r="65" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="199"/>
+      <c r="A65" s="206"/>
       <c r="B65" s="56"/>
-      <c r="C65" s="184"/>
+      <c r="C65" s="197"/>
       <c r="D65" s="12"/>
       <c r="E65" s="68"/>
       <c r="F65" s="66" t="s">
@@ -13620,9 +13620,9 @@
       <c r="BY65" s="10"/>
     </row>
     <row r="66" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="199"/>
+      <c r="A66" s="206"/>
       <c r="B66" s="56"/>
-      <c r="C66" s="184"/>
+      <c r="C66" s="197"/>
       <c r="D66" s="12"/>
       <c r="E66" s="68"/>
       <c r="F66" s="66" t="s">
@@ -13680,9 +13680,9 @@
       <c r="BY66" s="10"/>
     </row>
     <row r="67" spans="1:77" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="199"/>
+      <c r="A67" s="206"/>
       <c r="B67" s="56"/>
-      <c r="C67" s="184"/>
+      <c r="C67" s="197"/>
       <c r="D67" s="12"/>
       <c r="E67" s="68"/>
       <c r="F67" s="66" t="s">
@@ -13740,9 +13740,9 @@
       <c r="BY67" s="10"/>
     </row>
     <row r="68" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="201"/>
+      <c r="A68" s="207"/>
       <c r="B68" s="56"/>
-      <c r="C68" s="184" t="s">
+      <c r="C68" s="197" t="s">
         <v>39</v>
       </c>
       <c r="D68" s="12"/>
@@ -13803,9 +13803,9 @@
       </c>
     </row>
     <row r="69" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="201"/>
+      <c r="A69" s="207"/>
       <c r="B69" s="56"/>
-      <c r="C69" s="184"/>
+      <c r="C69" s="197"/>
       <c r="D69" s="12"/>
       <c r="E69" s="68"/>
       <c r="F69" s="127" t="s">
@@ -13854,7 +13854,7 @@
       <c r="AU69" s="6"/>
     </row>
     <row r="70" spans="1:77" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="201"/>
+      <c r="A70" s="207"/>
       <c r="B70" s="56"/>
       <c r="C70" s="14" t="s">
         <v>42</v>
@@ -13907,7 +13907,7 @@
       <c r="AU70" s="6"/>
     </row>
     <row r="71" spans="1:77" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="201"/>
+      <c r="A71" s="207"/>
       <c r="B71" s="56"/>
       <c r="C71" s="14" t="s">
         <v>44</v>
@@ -13960,9 +13960,9 @@
       <c r="AU71" s="6"/>
     </row>
     <row r="72" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="201"/>
+      <c r="A72" s="207"/>
       <c r="B72" s="56"/>
-      <c r="C72" s="184" t="s">
+      <c r="C72" s="197" t="s">
         <v>46</v>
       </c>
       <c r="D72" s="12"/>
@@ -14013,9 +14013,9 @@
       <c r="AU72" s="6"/>
     </row>
     <row r="73" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="201"/>
+      <c r="A73" s="207"/>
       <c r="B73" s="56"/>
-      <c r="C73" s="184"/>
+      <c r="C73" s="197"/>
       <c r="D73" s="12"/>
       <c r="E73" s="68"/>
       <c r="F73" s="128" t="s">
@@ -14064,9 +14064,9 @@
       <c r="AU73" s="6"/>
     </row>
     <row r="74" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="201"/>
+      <c r="A74" s="207"/>
       <c r="B74" s="56"/>
-      <c r="C74" s="184"/>
+      <c r="C74" s="197"/>
       <c r="D74" s="12"/>
       <c r="E74" s="68"/>
       <c r="F74" s="129" t="s">
@@ -14115,7 +14115,7 @@
       <c r="AU74" s="6"/>
     </row>
     <row r="75" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="201"/>
+      <c r="A75" s="207"/>
       <c r="B75" s="56"/>
       <c r="C75" s="14" t="s">
         <v>50</v>
@@ -14166,9 +14166,9 @@
       <c r="AU75" s="6"/>
     </row>
     <row r="76" spans="1:77" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="201"/>
+      <c r="A76" s="207"/>
       <c r="B76" s="56"/>
-      <c r="C76" s="185" t="s">
+      <c r="C76" s="221" t="s">
         <v>52</v>
       </c>
       <c r="D76" s="12"/>
@@ -14221,9 +14221,9 @@
       <c r="AU76" s="6"/>
     </row>
     <row r="77" spans="1:77" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="202"/>
+      <c r="A77" s="208"/>
       <c r="B77" s="29"/>
-      <c r="C77" s="186"/>
+      <c r="C77" s="222"/>
       <c r="D77" s="30"/>
       <c r="E77" s="79"/>
       <c r="F77" s="130" t="s">
@@ -14282,7 +14282,7 @@
       <c r="AU77" s="1"/>
     </row>
     <row r="78" spans="1:77" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="198" t="s">
+      <c r="A78" s="205" t="s">
         <v>191</v>
       </c>
       <c r="B78" s="27" t="s">
@@ -14347,7 +14347,7 @@
       <c r="AU78" s="1"/>
     </row>
     <row r="79" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="201" t="s">
+      <c r="A79" s="207" t="s">
         <v>57</v>
       </c>
       <c r="B79" s="56"/>
@@ -14406,7 +14406,7 @@
       <c r="AU79" s="1"/>
     </row>
     <row r="80" spans="1:77" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="201"/>
+      <c r="A80" s="207"/>
       <c r="B80" s="56" t="s">
         <v>59</v>
       </c>
@@ -14465,7 +14465,7 @@
       <c r="AU80" s="1"/>
     </row>
     <row r="81" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="201"/>
+      <c r="A81" s="207"/>
       <c r="B81" s="56"/>
       <c r="C81" s="14" t="s">
         <v>61</v>
@@ -14522,7 +14522,7 @@
       <c r="AU81" s="1"/>
     </row>
     <row r="82" spans="1:47" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="201"/>
+      <c r="A82" s="207"/>
       <c r="B82" s="56"/>
       <c r="C82" s="14" t="s">
         <v>122</v>
@@ -14579,7 +14579,7 @@
       <c r="AU82" s="1"/>
     </row>
     <row r="83" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A83" s="201"/>
+      <c r="A83" s="207"/>
       <c r="B83" s="80"/>
       <c r="C83" s="14" t="s">
         <v>123</v>
@@ -14634,7 +14634,7 @@
       <c r="AU83" s="1"/>
     </row>
     <row r="84" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A84" s="201"/>
+      <c r="A84" s="207"/>
       <c r="B84" s="80"/>
       <c r="C84" s="14" t="s">
         <v>124</v>
@@ -14689,7 +14689,7 @@
       <c r="AU84" s="1"/>
     </row>
     <row r="85" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A85" s="201"/>
+      <c r="A85" s="207"/>
       <c r="B85" s="80"/>
       <c r="C85" s="14" t="s">
         <v>125</v>
@@ -14744,7 +14744,7 @@
       <c r="AU85" s="1"/>
     </row>
     <row r="86" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A86" s="201"/>
+      <c r="A86" s="207"/>
       <c r="B86" s="80"/>
       <c r="C86" s="14" t="s">
         <v>126</v>
@@ -14799,7 +14799,7 @@
       <c r="AU86" s="1"/>
     </row>
     <row r="87" spans="1:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="201"/>
+      <c r="A87" s="207"/>
       <c r="B87" s="56"/>
       <c r="C87" s="14" t="s">
         <v>62</v>
@@ -14856,7 +14856,7 @@
       <c r="AU87" s="1"/>
     </row>
     <row r="88" spans="1:47" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="201"/>
+      <c r="A88" s="207"/>
       <c r="B88" s="56"/>
       <c r="C88" s="14" t="s">
         <v>63</v>
@@ -14911,7 +14911,7 @@
       <c r="AU88" s="1"/>
     </row>
     <row r="89" spans="1:47" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="201"/>
+      <c r="A89" s="207"/>
       <c r="B89" s="56"/>
       <c r="C89" s="14" t="s">
         <v>64</v>
@@ -14968,7 +14968,7 @@
       <c r="AU89" s="1"/>
     </row>
     <row r="90" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="201"/>
+      <c r="A90" s="207"/>
       <c r="B90" s="56" t="s">
         <v>65</v>
       </c>
@@ -15025,7 +15025,7 @@
       <c r="AU90" s="1"/>
     </row>
     <row r="91" spans="1:47" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="201"/>
+      <c r="A91" s="207"/>
       <c r="B91" s="56" t="s">
         <v>66</v>
       </c>
@@ -15082,7 +15082,7 @@
       <c r="AU91" s="1"/>
     </row>
     <row r="92" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A92" s="201"/>
+      <c r="A92" s="207"/>
       <c r="B92" s="84"/>
       <c r="C92" s="14" t="s">
         <v>142</v>
@@ -15131,7 +15131,7 @@
       <c r="AU92" s="1"/>
     </row>
     <row r="93" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A93" s="201"/>
+      <c r="A93" s="207"/>
       <c r="B93" s="84"/>
       <c r="C93" s="14" t="s">
         <v>143</v>
@@ -15180,7 +15180,7 @@
       <c r="AU93" s="1"/>
     </row>
     <row r="94" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="201"/>
+      <c r="A94" s="207"/>
       <c r="B94" s="56"/>
       <c r="C94" s="14" t="s">
         <v>144</v>
@@ -15235,7 +15235,7 @@
       <c r="AU94" s="1"/>
     </row>
     <row r="95" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="201"/>
+      <c r="A95" s="207"/>
       <c r="B95" s="56" t="s">
         <v>67</v>
       </c>
@@ -15292,7 +15292,7 @@
       <c r="AU95" s="1"/>
     </row>
     <row r="96" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="201"/>
+      <c r="A96" s="207"/>
       <c r="B96" s="56" t="s">
         <v>68</v>
       </c>
@@ -15349,7 +15349,7 @@
       <c r="AU96" s="1"/>
     </row>
     <row r="97" spans="1:47" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="201"/>
+      <c r="A97" s="207"/>
       <c r="B97" s="56" t="s">
         <v>69</v>
       </c>
@@ -15406,7 +15406,7 @@
       <c r="AU97" s="1"/>
     </row>
     <row r="98" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A98" s="201"/>
+      <c r="A98" s="207"/>
       <c r="B98" s="55" t="s">
         <v>70</v>
       </c>
@@ -15463,7 +15463,7 @@
       <c r="AU98" s="1"/>
     </row>
     <row r="99" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A99" s="201"/>
+      <c r="A99" s="207"/>
       <c r="B99" s="55" t="s">
         <v>70</v>
       </c>
@@ -15520,7 +15520,7 @@
       <c r="AU99" s="1"/>
     </row>
     <row r="100" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A100" s="201"/>
+      <c r="A100" s="207"/>
       <c r="B100" s="55" t="s">
         <v>70</v>
       </c>
@@ -15577,7 +15577,7 @@
       <c r="AU100" s="1"/>
     </row>
     <row r="101" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A101" s="201"/>
+      <c r="A101" s="207"/>
       <c r="B101" s="55" t="s">
         <v>70</v>
       </c>
@@ -15634,7 +15634,7 @@
       <c r="AU101" s="1"/>
     </row>
     <row r="102" spans="1:47" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="201"/>
+      <c r="A102" s="207"/>
       <c r="B102" s="55"/>
       <c r="C102" s="102"/>
       <c r="D102" s="48"/>
@@ -15689,10 +15689,10 @@
       <c r="AU102" s="1"/>
     </row>
     <row r="103" spans="1:47" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="203" t="s">
+      <c r="A103" s="187" t="s">
         <v>71</v>
       </c>
-      <c r="B103" s="181" t="s">
+      <c r="B103" s="218" t="s">
         <v>72</v>
       </c>
       <c r="C103" s="103" t="s">
@@ -15746,8 +15746,8 @@
       <c r="AU103" s="1"/>
     </row>
     <row r="104" spans="1:47" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="204"/>
-      <c r="B104" s="182"/>
+      <c r="A104" s="188"/>
+      <c r="B104" s="219"/>
       <c r="C104" s="104" t="s">
         <v>75</v>
       </c>
@@ -15799,8 +15799,8 @@
       <c r="AU104" s="1"/>
     </row>
     <row r="105" spans="1:47" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="204"/>
-      <c r="B105" s="182"/>
+      <c r="A105" s="188"/>
+      <c r="B105" s="219"/>
       <c r="C105" s="104" t="s">
         <v>77</v>
       </c>
@@ -15852,8 +15852,8 @@
       <c r="AU105" s="1"/>
     </row>
     <row r="106" spans="1:47" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="205"/>
-      <c r="B106" s="183"/>
+      <c r="A106" s="189"/>
+      <c r="B106" s="220"/>
       <c r="C106" s="105" t="s">
         <v>79</v>
       </c>
@@ -15905,7 +15905,7 @@
       <c r="AU106" s="1"/>
     </row>
     <row r="107" spans="1:47" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="206" t="s">
+      <c r="A107" s="199" t="s">
         <v>81</v>
       </c>
       <c r="B107" s="73" t="s">
@@ -15935,7 +15935,7 @@
       <c r="S107" s="25"/>
     </row>
     <row r="108" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="207"/>
+      <c r="A108" s="200"/>
       <c r="B108" s="70"/>
       <c r="C108" s="3" t="s">
         <v>84</v>
@@ -15961,7 +15961,7 @@
       <c r="S108" s="25"/>
     </row>
     <row r="109" spans="1:47" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="196" t="s">
+      <c r="A109" s="185" t="s">
         <v>85</v>
       </c>
       <c r="B109" s="70"/>
@@ -15989,7 +15989,7 @@
       <c r="S109" s="25"/>
     </row>
     <row r="110" spans="1:47" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="196"/>
+      <c r="A110" s="185"/>
       <c r="B110" s="70"/>
       <c r="C110" s="3" t="s">
         <v>87</v>
@@ -16015,7 +16015,7 @@
       <c r="S110" s="25"/>
     </row>
     <row r="111" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A111" s="196"/>
+      <c r="A111" s="185"/>
       <c r="B111" s="70"/>
       <c r="C111" s="107" t="s">
         <v>88</v>
@@ -16039,7 +16039,7 @@
       <c r="S111" s="25"/>
     </row>
     <row r="112" spans="1:47" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="196"/>
+      <c r="A112" s="185"/>
       <c r="B112" s="70"/>
       <c r="C112" s="3" t="s">
         <v>89</v>
@@ -16065,7 +16065,7 @@
       <c r="S112" s="25"/>
     </row>
     <row r="113" spans="1:44" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="196"/>
+      <c r="A113" s="185"/>
       <c r="B113" s="70"/>
       <c r="C113" s="3" t="s">
         <v>90</v>
@@ -16091,7 +16091,7 @@
       <c r="S113" s="25"/>
     </row>
     <row r="114" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A114" s="196"/>
+      <c r="A114" s="185"/>
       <c r="B114" s="70"/>
       <c r="C114" s="107" t="s">
         <v>91</v>
@@ -16115,7 +16115,7 @@
       <c r="S114" s="25"/>
     </row>
     <row r="115" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="196"/>
+      <c r="A115" s="185"/>
       <c r="B115" s="70"/>
       <c r="C115" s="3" t="s">
         <v>92</v>
@@ -16141,7 +16141,7 @@
       <c r="S115" s="25"/>
     </row>
     <row r="116" spans="1:44" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="196"/>
+      <c r="A116" s="185"/>
       <c r="B116" s="70"/>
       <c r="C116" s="3" t="s">
         <v>93</v>
@@ -16167,7 +16167,7 @@
       <c r="S116" s="25"/>
     </row>
     <row r="117" spans="1:44" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="208"/>
+      <c r="A117" s="201"/>
       <c r="B117" s="70"/>
       <c r="C117" s="3" t="s">
         <v>94</v>
@@ -16193,7 +16193,7 @@
       <c r="S117" s="25"/>
     </row>
     <row r="118" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="208"/>
+      <c r="A118" s="201"/>
       <c r="B118" s="70" t="s">
         <v>95</v>
       </c>
@@ -16221,7 +16221,7 @@
       <c r="S118" s="25"/>
     </row>
     <row r="119" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="208"/>
+      <c r="A119" s="201"/>
       <c r="B119" s="70"/>
       <c r="C119" s="3" t="s">
         <v>90</v>
@@ -16247,7 +16247,7 @@
       <c r="S119" s="25"/>
     </row>
     <row r="120" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A120" s="208"/>
+      <c r="A120" s="201"/>
       <c r="B120" s="70"/>
       <c r="C120" s="107" t="s">
         <v>91</v>
@@ -16271,7 +16271,7 @@
       <c r="S120" s="25"/>
     </row>
     <row r="121" spans="1:44" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="208"/>
+      <c r="A121" s="201"/>
       <c r="B121" s="70"/>
       <c r="C121" s="3" t="s">
         <v>92</v>
@@ -16297,7 +16297,7 @@
       <c r="S121" s="25"/>
     </row>
     <row r="122" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="208"/>
+      <c r="A122" s="201"/>
       <c r="B122" s="70"/>
       <c r="C122" s="3" t="s">
         <v>93</v>
@@ -16323,7 +16323,7 @@
       <c r="S122" s="25"/>
     </row>
     <row r="123" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="208"/>
+      <c r="A123" s="201"/>
       <c r="B123" s="70"/>
       <c r="C123" s="3" t="s">
         <v>94</v>
@@ -16349,7 +16349,7 @@
       <c r="S123" s="25"/>
     </row>
     <row r="124" spans="1:44" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="208"/>
+      <c r="A124" s="201"/>
       <c r="B124" s="70"/>
       <c r="C124" s="9" t="s">
         <v>148</v>
@@ -16376,7 +16376,7 @@
       <c r="S124" s="25"/>
     </row>
     <row r="125" spans="1:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="208"/>
+      <c r="A125" s="201"/>
       <c r="B125" s="70"/>
       <c r="C125" s="9" t="s">
         <v>149</v>
@@ -16403,7 +16403,7 @@
       <c r="S125" s="25"/>
     </row>
     <row r="126" spans="1:44" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="208"/>
+      <c r="A126" s="201"/>
       <c r="B126" s="70"/>
       <c r="C126" s="9" t="s">
         <v>150</v>
@@ -16430,7 +16430,7 @@
       <c r="S126" s="25"/>
     </row>
     <row r="127" spans="1:44" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="208"/>
+      <c r="A127" s="201"/>
       <c r="B127" s="70" t="s">
         <v>96</v>
       </c>
@@ -16482,7 +16482,7 @@
       <c r="AR127" s="101"/>
     </row>
     <row r="128" spans="1:44" s="31" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="208"/>
+      <c r="A128" s="201"/>
       <c r="B128" s="70" t="s">
         <v>97</v>
       </c>
@@ -16536,7 +16536,7 @@
       <c r="AR128" s="101"/>
     </row>
     <row r="129" spans="1:47" s="26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="208"/>
+      <c r="A129" s="201"/>
       <c r="B129" s="70" t="s">
         <v>98</v>
       </c>
@@ -16590,7 +16590,7 @@
       <c r="AR129" s="101"/>
     </row>
     <row r="130" spans="1:47" s="26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="208"/>
+      <c r="A130" s="201"/>
       <c r="B130" s="70" t="s">
         <v>194</v>
       </c>
@@ -16640,7 +16640,7 @@
       <c r="AR130" s="106"/>
     </row>
     <row r="131" spans="1:47" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="208"/>
+      <c r="A131" s="201"/>
       <c r="B131" s="70" t="s">
         <v>99</v>
       </c>
@@ -16692,17 +16692,17 @@
       <c r="AR131" s="101"/>
     </row>
     <row r="132" spans="1:47" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="209"/>
-      <c r="B132" s="211" t="s">
+      <c r="A132" s="202"/>
+      <c r="B132" s="173" t="s">
         <v>100</v>
       </c>
       <c r="C132" s="47"/>
       <c r="D132" s="47"/>
-      <c r="E132" s="212"/>
+      <c r="E132" s="174"/>
       <c r="F132" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="G132" s="220"/>
+      <c r="G132" s="179"/>
       <c r="H132" s="47"/>
       <c r="I132" s="47"/>
       <c r="J132" s="47"/>
@@ -16746,21 +16746,19 @@
       <c r="AR132" s="101"/>
     </row>
     <row r="133" spans="1:47" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="213" t="s">
+      <c r="A133" s="182" t="s">
         <v>195</v>
       </c>
-      <c r="B133" s="216" t="s">
+      <c r="B133" s="175" t="s">
         <v>196</v>
       </c>
       <c r="C133" s="152"/>
       <c r="D133" s="139"/>
       <c r="E133" s="149"/>
-      <c r="F133" s="195" t="s">
+      <c r="F133" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="G133" s="36" t="s">
-        <v>19</v>
-      </c>
+      <c r="G133" s="36"/>
       <c r="H133" s="139"/>
       <c r="I133" s="139"/>
       <c r="J133" s="139"/>
@@ -16769,7 +16767,9 @@
       <c r="M133" s="36"/>
       <c r="N133" s="36"/>
       <c r="O133" s="35"/>
-      <c r="P133" s="34"/>
+      <c r="P133" s="36" t="s">
+        <v>19</v>
+      </c>
       <c r="Q133" s="34"/>
       <c r="R133" s="140"/>
       <c r="S133" s="33"/>
@@ -16801,19 +16801,17 @@
       <c r="AU133" s="1"/>
     </row>
     <row r="134" spans="1:47" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="214"/>
-      <c r="B134" s="217" t="s">
+      <c r="A134" s="183"/>
+      <c r="B134" s="176" t="s">
         <v>197</v>
       </c>
       <c r="C134" s="151"/>
       <c r="D134" s="22"/>
       <c r="E134" s="150"/>
-      <c r="F134" s="195" t="s">
+      <c r="F134" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="G134" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G134" s="5"/>
       <c r="H134" s="22"/>
       <c r="I134" s="22"/>
       <c r="J134" s="22"/>
@@ -16822,7 +16820,9 @@
       <c r="M134" s="5"/>
       <c r="N134" s="5"/>
       <c r="O134" s="6"/>
-      <c r="P134" s="1"/>
+      <c r="P134" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q134" s="1"/>
       <c r="R134" s="54"/>
       <c r="S134" s="33"/>
@@ -16854,19 +16854,17 @@
       <c r="AU134" s="1"/>
     </row>
     <row r="135" spans="1:47" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="214"/>
-      <c r="B135" s="217" t="s">
+      <c r="A135" s="183"/>
+      <c r="B135" s="176" t="s">
         <v>198</v>
       </c>
       <c r="C135" s="151"/>
       <c r="D135" s="22"/>
       <c r="E135" s="150"/>
-      <c r="F135" s="195" t="s">
+      <c r="F135" s="171" t="s">
         <v>78</v>
       </c>
-      <c r="G135" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G135" s="5"/>
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
@@ -16875,7 +16873,9 @@
       <c r="M135" s="5"/>
       <c r="N135" s="5"/>
       <c r="O135" s="6"/>
-      <c r="P135" s="1"/>
+      <c r="P135" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q135" s="1"/>
       <c r="R135" s="54"/>
       <c r="S135" s="33"/>
@@ -16907,19 +16907,17 @@
       <c r="AU135" s="1"/>
     </row>
     <row r="136" spans="1:47" s="23" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="214"/>
-      <c r="B136" s="217" t="s">
+      <c r="A136" s="183"/>
+      <c r="B136" s="176" t="s">
         <v>199</v>
       </c>
       <c r="C136" s="151"/>
       <c r="D136" s="22"/>
       <c r="E136" s="150"/>
-      <c r="F136" s="195" t="s">
+      <c r="F136" s="171" t="s">
         <v>80</v>
       </c>
-      <c r="G136" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G136" s="5"/>
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
       <c r="J136" s="1"/>
@@ -16928,7 +16926,9 @@
       <c r="M136" s="5"/>
       <c r="N136" s="5"/>
       <c r="O136" s="6"/>
-      <c r="P136" s="1"/>
+      <c r="P136" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q136" s="1"/>
       <c r="R136" s="54"/>
       <c r="S136" s="33"/>
@@ -16960,17 +16960,15 @@
       <c r="AU136" s="1"/>
     </row>
     <row r="137" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A137" s="214"/>
-      <c r="B137" s="217" t="s">
+      <c r="A137" s="183"/>
+      <c r="B137" s="176" t="s">
         <v>200</v>
       </c>
       <c r="C137" s="153"/>
       <c r="D137" s="153"/>
       <c r="E137" s="71"/>
       <c r="F137" s="145"/>
-      <c r="G137" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G137" s="5"/>
       <c r="H137" s="153"/>
       <c r="I137" s="153"/>
       <c r="J137" s="153"/>
@@ -16979,9 +16977,11 @@
       <c r="M137" s="153"/>
       <c r="N137" s="153"/>
       <c r="O137" s="153"/>
-      <c r="P137" s="153"/>
+      <c r="P137" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q137" s="153"/>
-      <c r="R137" s="221"/>
+      <c r="R137" s="180"/>
       <c r="S137" s="25"/>
       <c r="T137" s="101"/>
       <c r="U137" s="101"/>
@@ -17010,17 +17010,15 @@
       <c r="AR137" s="101"/>
     </row>
     <row r="138" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A138" s="214"/>
-      <c r="B138" s="217" t="s">
+      <c r="A138" s="183"/>
+      <c r="B138" s="176" t="s">
         <v>201</v>
       </c>
       <c r="C138" s="153"/>
       <c r="D138" s="153"/>
       <c r="E138" s="71"/>
       <c r="F138" s="145"/>
-      <c r="G138" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G138" s="5"/>
       <c r="H138" s="153"/>
       <c r="I138" s="153"/>
       <c r="J138" s="153"/>
@@ -17029,9 +17027,11 @@
       <c r="M138" s="153"/>
       <c r="N138" s="153"/>
       <c r="O138" s="153"/>
-      <c r="P138" s="153"/>
+      <c r="P138" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q138" s="153"/>
-      <c r="R138" s="221"/>
+      <c r="R138" s="180"/>
       <c r="S138" s="25"/>
       <c r="T138" s="101"/>
       <c r="U138" s="101"/>
@@ -17060,17 +17060,15 @@
       <c r="AR138" s="101"/>
     </row>
     <row r="139" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A139" s="214"/>
-      <c r="B139" s="217" t="s">
+      <c r="A139" s="183"/>
+      <c r="B139" s="176" t="s">
         <v>202</v>
       </c>
       <c r="C139" s="153"/>
       <c r="D139" s="153"/>
       <c r="E139" s="71"/>
       <c r="F139" s="145"/>
-      <c r="G139" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G139" s="5"/>
       <c r="H139" s="153"/>
       <c r="I139" s="153"/>
       <c r="J139" s="153"/>
@@ -17079,9 +17077,11 @@
       <c r="M139" s="153"/>
       <c r="N139" s="153"/>
       <c r="O139" s="153"/>
-      <c r="P139" s="153"/>
+      <c r="P139" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q139" s="153"/>
-      <c r="R139" s="221"/>
+      <c r="R139" s="180"/>
       <c r="S139" s="25"/>
       <c r="T139" s="101"/>
       <c r="U139" s="101"/>
@@ -17110,17 +17110,15 @@
       <c r="AR139" s="101"/>
     </row>
     <row r="140" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A140" s="214"/>
-      <c r="B140" s="218" t="s">
+      <c r="A140" s="183"/>
+      <c r="B140" s="177" t="s">
         <v>203</v>
       </c>
       <c r="C140" s="153"/>
       <c r="D140" s="153"/>
       <c r="E140" s="71"/>
       <c r="F140" s="145"/>
-      <c r="G140" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G140" s="5"/>
       <c r="H140" s="153"/>
       <c r="I140" s="153"/>
       <c r="J140" s="153"/>
@@ -17129,9 +17127,11 @@
       <c r="M140" s="153"/>
       <c r="N140" s="153"/>
       <c r="O140" s="153"/>
-      <c r="P140" s="153"/>
+      <c r="P140" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q140" s="153"/>
-      <c r="R140" s="221"/>
+      <c r="R140" s="180"/>
       <c r="S140" s="25"/>
       <c r="T140" s="101"/>
       <c r="U140" s="101"/>
@@ -17160,17 +17160,15 @@
       <c r="AR140" s="101"/>
     </row>
     <row r="141" spans="1:47" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="214"/>
-      <c r="B141" s="217" t="s">
+      <c r="A141" s="183"/>
+      <c r="B141" s="176" t="s">
         <v>205</v>
       </c>
       <c r="C141" s="153"/>
       <c r="D141" s="153"/>
       <c r="E141" s="71"/>
       <c r="F141" s="145"/>
-      <c r="G141" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G141" s="5"/>
       <c r="H141" s="153"/>
       <c r="I141" s="153"/>
       <c r="J141" s="153"/>
@@ -17179,9 +17177,11 @@
       <c r="M141" s="153"/>
       <c r="N141" s="153"/>
       <c r="O141" s="153"/>
-      <c r="P141" s="153"/>
+      <c r="P141" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q141" s="153"/>
-      <c r="R141" s="221"/>
+      <c r="R141" s="180"/>
       <c r="S141" s="25"/>
       <c r="T141" s="101"/>
       <c r="U141" s="101"/>
@@ -17210,17 +17210,15 @@
       <c r="AR141" s="101"/>
     </row>
     <row r="142" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A142" s="214"/>
-      <c r="B142" s="217" t="s">
+      <c r="A142" s="183"/>
+      <c r="B142" s="176" t="s">
         <v>204</v>
       </c>
       <c r="C142" s="153"/>
       <c r="D142" s="153"/>
       <c r="E142" s="71"/>
       <c r="F142" s="145"/>
-      <c r="G142" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G142" s="5"/>
       <c r="H142" s="153"/>
       <c r="I142" s="153"/>
       <c r="J142" s="153"/>
@@ -17229,9 +17227,11 @@
       <c r="M142" s="153"/>
       <c r="N142" s="153"/>
       <c r="O142" s="153"/>
-      <c r="P142" s="153"/>
+      <c r="P142" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q142" s="153"/>
-      <c r="R142" s="221"/>
+      <c r="R142" s="180"/>
       <c r="S142" s="25"/>
       <c r="T142" s="101"/>
       <c r="U142" s="101"/>
@@ -17260,17 +17260,15 @@
       <c r="AR142" s="101"/>
     </row>
     <row r="143" spans="1:47" ht="30" x14ac:dyDescent="0.25">
-      <c r="A143" s="214"/>
-      <c r="B143" s="217" t="s">
+      <c r="A143" s="183"/>
+      <c r="B143" s="176" t="s">
         <v>206</v>
       </c>
       <c r="C143" s="153"/>
       <c r="D143" s="153"/>
       <c r="E143" s="71"/>
       <c r="F143" s="145"/>
-      <c r="G143" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="G143" s="5"/>
       <c r="H143" s="153"/>
       <c r="I143" s="153"/>
       <c r="J143" s="153"/>
@@ -17279,9 +17277,11 @@
       <c r="M143" s="153"/>
       <c r="N143" s="153"/>
       <c r="O143" s="153"/>
-      <c r="P143" s="153"/>
+      <c r="P143" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="Q143" s="153"/>
-      <c r="R143" s="221"/>
+      <c r="R143" s="180"/>
       <c r="S143" s="25"/>
       <c r="T143" s="101"/>
       <c r="U143" s="101"/>
@@ -17310,17 +17310,15 @@
       <c r="AR143" s="101"/>
     </row>
     <row r="144" spans="1:47" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="215"/>
-      <c r="B144" s="219" t="s">
+      <c r="A144" s="184"/>
+      <c r="B144" s="178" t="s">
         <v>207</v>
       </c>
       <c r="C144" s="154"/>
       <c r="D144" s="154"/>
       <c r="E144" s="72"/>
       <c r="F144" s="145"/>
-      <c r="G144" s="170" t="s">
-        <v>19</v>
-      </c>
+      <c r="G144" s="170"/>
       <c r="H144" s="154"/>
       <c r="I144" s="154"/>
       <c r="J144" s="154"/>
@@ -17329,9 +17327,11 @@
       <c r="M144" s="154"/>
       <c r="N144" s="154"/>
       <c r="O144" s="154"/>
-      <c r="P144" s="154"/>
+      <c r="P144" s="170" t="s">
+        <v>19</v>
+      </c>
       <c r="Q144" s="154"/>
-      <c r="R144" s="222"/>
+      <c r="R144" s="181"/>
       <c r="S144" s="25"/>
       <c r="T144" s="101"/>
       <c r="U144" s="101"/>
@@ -17993,32 +17993,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A133:A144"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="A107:A132"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="A55:A77"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A78:A102"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A14:A54"/>
     <mergeCell ref="G1:O1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B103:B106"/>
     <mergeCell ref="C68:C69"/>
     <mergeCell ref="C76:C77"/>
     <mergeCell ref="C72:C74"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="A133:A144"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A107:A132"/>
+    <mergeCell ref="A78:A102"/>
+    <mergeCell ref="B103:B106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F103:F106" r:id="rId1" location="2932-manual-adjudication-decision-service" display="POST /registration-processor/manual-adjudication/assignment" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -18053,12 +18053,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18269,35 +18286,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85E73B9D-1766-405A-9B26-47DF7884A997}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B443FFFF-5AD5-4D1A-BEBD-F002358985A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18322,12 +18325,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B443FFFF-5AD5-4D1A-BEBD-F002358985A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85E73B9D-1766-405A-9B26-47DF7884A997}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>